<commit_message>
dashboards adicionados e validação de e-mail incluida no cadastro
</commit_message>
<xml_diff>
--- a/Documentacao/Sprint 2/Métricas/Métricas HF System.xlsx
+++ b/Documentacao/Sprint 2/Métricas/Métricas HF System.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicol\Downloads\SPtech\HFSystem\Documentacao\Sprint 2\Métricas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e27a146a09249998/Área de Trabalho/HFSystem/Documentacao/Sprint 2/Métricas/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="8_{48C030F4-087A-45DB-8174-2DB6DE11F5C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{8F95BAA1-0D4E-4381-AD42-20580717B913}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="20640" windowHeight="11040" activeTab="1" xr2:uid="{8F95BAA1-0D4E-4381-AD42-20580717B913}"/>
   </bookViews>
   <sheets>
     <sheet name="Dados" sheetId="1" r:id="rId1"/>
@@ -4149,8 +4149,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82BC690B-CE3C-4AAF-B63F-4FE30B4A4D5F}">
   <dimension ref="C3:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4217,6 +4217,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="9fdc8751-6fef-42ec-b05c-835dd8c535b4" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FD11765F9AC0004AAF0A4CAAFDFAF16A" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="86c5ac76e231860da655e5933d23dd68">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="9fdc8751-6fef-42ec-b05c-835dd8c535b4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1f4f46dfd8bb482fb70daaaaafa182ce" ns3:_="">
     <xsd:import namespace="9fdc8751-6fef-42ec-b05c-835dd8c535b4"/>
@@ -4372,24 +4389,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F11B4C93-784F-47FD-8FBA-CE323522DE73}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="9fdc8751-6fef-42ec-b05c-835dd8c535b4"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="9fdc8751-6fef-42ec-b05c-835dd8c535b4" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{05D78DEA-8933-4A88-881F-E77ECC750FD0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1032FB05-B4FC-4968-8C30-8572B30A507C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4405,28 +4429,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{05D78DEA-8933-4A88-881F-E77ECC750FD0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F11B4C93-784F-47FD-8FBA-CE323522DE73}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="9fdc8751-6fef-42ec-b05c-835dd8c535b4"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>